<commit_message>
Modified data model, added API's for cpt_categories, cpt_codes, disorders, diagnosis_codes and episodes_of_care
</commit_message>
<xml_diff>
--- a/data/cpt_codes.xlsx
+++ b/data/cpt_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelinn/dev/OutcomesAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B14ACFDF-0841-7442-B70B-149FF89660D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E160E1D8-531A-BB4D-903D-CDED6442880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3500" windowWidth="26440" windowHeight="15440" xr2:uid="{FD5FDCDF-47C4-6245-9B83-B436BDCE5A1A}"/>
+    <workbookView xWindow="4580" yWindow="1580" windowWidth="21440" windowHeight="15440" xr2:uid="{FD5FDCDF-47C4-6245-9B83-B436BDCE5A1A}"/>
   </bookViews>
   <sheets>
     <sheet name="cpt_codes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -44,24 +44,15 @@
     <t>code</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>Initial Evaluation</t>
-  </si>
-  <si>
     <t>Psychiatric Diagnostic Evaluation without medical services</t>
   </si>
   <si>
     <t>Psychiatric Diagnostic Evaluation with medical services</t>
   </si>
   <si>
-    <t>Psychotherapy</t>
-  </si>
-  <si>
     <t>Psychotherapy 30 minutes</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>90846</t>
   </si>
   <si>
-    <t>Family Psychotherapy</t>
-  </si>
-  <si>
     <t>Family psychotherapy (without the patient present) 50 minutes</t>
   </si>
   <si>
@@ -110,24 +98,15 @@
     <t>90853</t>
   </si>
   <si>
-    <t>Group Psychotherapy</t>
-  </si>
-  <si>
     <t>Group psychotherapy (other than of a multiple-family group)</t>
   </si>
   <si>
     <t>90863</t>
   </si>
   <si>
-    <t>Pharmacologic Management</t>
-  </si>
-  <si>
     <t>Pharmacologic management including prescription and review of medication when performed with psychotherapy services</t>
   </si>
   <si>
-    <t>TMS</t>
-  </si>
-  <si>
     <t>Therapeutic repetitive transcranial magnetic stimulation (TMS) initial</t>
   </si>
   <si>
@@ -137,9 +116,6 @@
     <t>Therapeutic repetitive transcranial magnetic stimulation (TMS) subsequent motor threshold re-determination with delivery and management</t>
   </si>
   <si>
-    <t>Biofeedback</t>
-  </si>
-  <si>
     <t>Individual psychophysiological therapy incorporating biofeedback training 30 minutes</t>
   </si>
   <si>
@@ -161,15 +137,6 @@
     <t>Biofeedback train additional 15 minutes</t>
   </si>
   <si>
-    <t>New Patient Office Visit</t>
-  </si>
-  <si>
-    <t>Established Patient Office Visit</t>
-  </si>
-  <si>
-    <t>Telephone Established Patient</t>
-  </si>
-  <si>
     <t>Psychotherapy 30 minutes with EM service</t>
   </si>
   <si>
@@ -216,6 +183,15 @@
   </si>
   <si>
     <t>Telephone EM service provided to an established patient-parent-guardian 21-30 minutes</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -579,21 +555,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF49FBD9-3B3D-B048-8AFF-BD38EFD34A4B}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A12" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="120.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,528 +577,642 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>90791</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="C2" s="1">
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>90792</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>90832</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="1">
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>90833</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
+      <c r="C5" s="1">
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>90834</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
+      <c r="C6" s="1">
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>90836</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
+      <c r="C7" s="1">
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>90837</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>90838</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
+      <c r="C9" s="1">
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>90839</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
+      <c r="C10" s="1">
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>90867</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
+      <c r="C18" s="1">
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>90868</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
+      <c r="C19" s="1">
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>90869</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
+      <c r="C20" s="1">
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="3">
         <v>90875</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
+      <c r="C21" s="1">
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>90880</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>35</v>
+      <c r="C22" s="1">
+        <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>90901</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>33</v>
+      <c r="C23" s="1">
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>99201</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>41</v>
+      <c r="C26" s="1">
+        <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="3">
         <v>99202</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>41</v>
+      <c r="C27" s="1">
+        <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>99203</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>41</v>
+      <c r="C28" s="1">
+        <v>9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>99204</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>41</v>
+      <c r="C29" s="1">
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>99205</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>41</v>
+      <c r="C30" s="1">
+        <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="3">
         <v>99211</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
+      <c r="C31" s="1">
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="3">
         <v>99212</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="3">
         <v>99213</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
+      <c r="C33" s="1">
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>99214</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>42</v>
+      <c r="C34" s="1">
+        <v>10</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="3">
         <v>99215</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
+      <c r="C35" s="1">
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>99441</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>43</v>
+      <c r="C36" s="1">
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="3">
         <v>99442</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
+      <c r="C37" s="1">
+        <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="3">
         <v>99443</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>43</v>
+      <c r="C38" s="1">
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+      <c r="E38" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>